<commit_message>
Adding English Champs 2022
</commit_message>
<xml_diff>
--- a/FIG-2022-Score-Comparison.xlsx
+++ b/FIG-2022-Score-Comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="41">
   <si>
     <t>Av Vault</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Floor Finals</t>
   </si>
   <si>
-    <t xml:space="preserve">Floor </t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -100,12 +97,6 @@
     <t>Junior WAG Beam Final</t>
   </si>
   <si>
-    <t>Senior WAG Beam AA</t>
-  </si>
-  <si>
-    <t>Junior WAG Beam AA</t>
-  </si>
-  <si>
     <t>Overall - WAG</t>
   </si>
   <si>
@@ -134,13 +125,35 @@
   </si>
   <si>
     <t>2019: https://www.gymdata.co.uk/events/download-documents.aspx?eid=912</t>
+  </si>
+  <si>
+    <t>Senior WAG
+Beam Final</t>
+  </si>
+  <si>
+    <t>NOT AVAILABLE</t>
+  </si>
+  <si>
+    <t>MAG Senior Floor</t>
+  </si>
+  <si>
+    <t>MAG Junior Floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senior WAG Beam </t>
+  </si>
+  <si>
+    <t>Junior WAG Beam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +197,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -221,12 +239,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -238,7 +271,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -263,6 +296,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -551,13 +587,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E163" sqref="E163"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
   </cols>
@@ -634,7 +674,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -664,12 +704,12 @@
         <v>2022</v>
       </c>
       <c r="H17" s="1">
-        <v>20022</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -713,6 +753,12 @@
       <c r="B21">
         <v>12.9</v>
       </c>
+      <c r="D21">
+        <v>13.55</v>
+      </c>
+      <c r="E21">
+        <v>12.95</v>
+      </c>
       <c r="G21">
         <v>13.8</v>
       </c>
@@ -727,6 +773,12 @@
       <c r="B22">
         <v>12.534000000000001</v>
       </c>
+      <c r="D22">
+        <v>13.2</v>
+      </c>
+      <c r="E22">
+        <v>12.7</v>
+      </c>
       <c r="G22">
         <v>13.05</v>
       </c>
@@ -741,6 +793,12 @@
       <c r="B23">
         <v>12.467000000000001</v>
       </c>
+      <c r="D23">
+        <v>13.45</v>
+      </c>
+      <c r="E23">
+        <v>11.85</v>
+      </c>
       <c r="G23">
         <v>12.45</v>
       </c>
@@ -755,6 +813,12 @@
       <c r="B24">
         <v>12.266999999999999</v>
       </c>
+      <c r="D24">
+        <v>13.35</v>
+      </c>
+      <c r="E24">
+        <v>11.95</v>
+      </c>
       <c r="G24">
         <v>13.05</v>
       </c>
@@ -769,6 +833,12 @@
       <c r="B25">
         <v>12.534000000000001</v>
       </c>
+      <c r="D25">
+        <v>13.15</v>
+      </c>
+      <c r="E25">
+        <v>12.45</v>
+      </c>
       <c r="G25">
         <v>11.65</v>
       </c>
@@ -783,6 +853,12 @@
       <c r="B26">
         <v>11.266999999999999</v>
       </c>
+      <c r="D26">
+        <v>13</v>
+      </c>
+      <c r="E26">
+        <v>11.45</v>
+      </c>
       <c r="G26">
         <v>11.5</v>
       </c>
@@ -797,6 +873,12 @@
       <c r="B27">
         <v>12.567</v>
       </c>
+      <c r="D27">
+        <v>12.5</v>
+      </c>
+      <c r="E27">
+        <v>12.25</v>
+      </c>
       <c r="G27">
         <v>11.95</v>
       </c>
@@ -811,6 +893,12 @@
       <c r="B28">
         <v>12.5</v>
       </c>
+      <c r="D28">
+        <v>12.4</v>
+      </c>
+      <c r="E28">
+        <v>11.7</v>
+      </c>
       <c r="G28">
         <v>12.2</v>
       </c>
@@ -825,6 +913,12 @@
       <c r="B29">
         <v>11.034000000000001</v>
       </c>
+      <c r="D29">
+        <v>12.7</v>
+      </c>
+      <c r="E29">
+        <v>12.1</v>
+      </c>
       <c r="G29">
         <v>12.05</v>
       </c>
@@ -839,6 +933,12 @@
       <c r="B30">
         <v>11.266999999999999</v>
       </c>
+      <c r="D30">
+        <v>11.9</v>
+      </c>
+      <c r="E30">
+        <v>12.8</v>
+      </c>
       <c r="G30">
         <v>11.85</v>
       </c>
@@ -853,6 +953,12 @@
       <c r="B31">
         <v>12.5</v>
       </c>
+      <c r="D31">
+        <v>12</v>
+      </c>
+      <c r="E31">
+        <v>12.35</v>
+      </c>
       <c r="G31">
         <v>11.2</v>
       </c>
@@ -867,6 +973,12 @@
       <c r="B32">
         <v>12.2</v>
       </c>
+      <c r="D32">
+        <v>12.4</v>
+      </c>
+      <c r="E32">
+        <v>11.05</v>
+      </c>
       <c r="G32">
         <v>12.6</v>
       </c>
@@ -881,6 +993,12 @@
       <c r="B33">
         <v>11.4</v>
       </c>
+      <c r="D33">
+        <v>11.8</v>
+      </c>
+      <c r="E33">
+        <v>11.5</v>
+      </c>
       <c r="G33">
         <v>11.7</v>
       </c>
@@ -892,6 +1010,9 @@
       <c r="B34">
         <v>12.2</v>
       </c>
+      <c r="D34">
+        <v>12.25</v>
+      </c>
       <c r="G34">
         <v>11.55</v>
       </c>
@@ -903,6 +1024,9 @@
       <c r="B35">
         <v>11.034000000000001</v>
       </c>
+      <c r="D35">
+        <v>10.6</v>
+      </c>
       <c r="G35">
         <v>11.95</v>
       </c>
@@ -913,6 +1037,9 @@
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>10.9</v>
+      </c>
+      <c r="D36">
+        <v>12.35</v>
       </c>
       <c r="G36">
         <v>11.7</v>
@@ -1005,8 +1132,12 @@
         <v>0</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
         <v>16</v>
@@ -1022,6 +1153,12 @@
       <c r="B46">
         <v>12.525</v>
       </c>
+      <c r="D46">
+        <v>12.95</v>
+      </c>
+      <c r="E46">
+        <v>12.55</v>
+      </c>
       <c r="G46">
         <v>12.867000000000001</v>
       </c>
@@ -1036,6 +1173,12 @@
       <c r="B47">
         <v>12.525</v>
       </c>
+      <c r="D47">
+        <v>12.725</v>
+      </c>
+      <c r="E47">
+        <v>12.45</v>
+      </c>
       <c r="G47">
         <v>12.417</v>
       </c>
@@ -1050,6 +1193,12 @@
       <c r="B48">
         <v>12.375</v>
       </c>
+      <c r="D48">
+        <v>12.7</v>
+      </c>
+      <c r="E48">
+        <v>12.275</v>
+      </c>
       <c r="G48">
         <v>12.284000000000001</v>
       </c>
@@ -1064,6 +1213,12 @@
       <c r="B49">
         <v>12.35</v>
       </c>
+      <c r="D49">
+        <v>12.65</v>
+      </c>
+      <c r="E49">
+        <v>12.25</v>
+      </c>
       <c r="G49">
         <v>12.266999999999999</v>
       </c>
@@ -1078,6 +1233,12 @@
       <c r="B50">
         <v>12.35</v>
       </c>
+      <c r="D50">
+        <v>12.525</v>
+      </c>
+      <c r="E50">
+        <v>12.175000000000001</v>
+      </c>
       <c r="G50">
         <v>11.85</v>
       </c>
@@ -1092,6 +1253,12 @@
       <c r="B51">
         <v>12.275</v>
       </c>
+      <c r="D51">
+        <v>11.35</v>
+      </c>
+      <c r="E51">
+        <v>12.1</v>
+      </c>
       <c r="G51">
         <v>11.516999999999999</v>
       </c>
@@ -1106,6 +1273,9 @@
       <c r="B52">
         <v>12.275</v>
       </c>
+      <c r="E52">
+        <v>12</v>
+      </c>
       <c r="G52">
         <v>11.266999999999999</v>
       </c>
@@ -1119,6 +1289,9 @@
       </c>
       <c r="B53">
         <v>12.125</v>
+      </c>
+      <c r="E53">
+        <v>5.9249999999999998</v>
       </c>
       <c r="G53">
         <v>6.3</v>
@@ -1170,22 +1343,36 @@
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
     </row>
-    <row r="59" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2018</v>
+      </c>
+      <c r="D59">
+        <v>2019</v>
+      </c>
+      <c r="G59">
+        <v>2022</v>
+      </c>
+    </row>
     <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
+      <c r="D60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="G60" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H60" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -1195,6 +1382,12 @@
       <c r="B61">
         <v>12.4</v>
       </c>
+      <c r="D61">
+        <v>13.2</v>
+      </c>
+      <c r="E61">
+        <v>12.5</v>
+      </c>
       <c r="G61">
         <v>12.4</v>
       </c>
@@ -1209,6 +1402,12 @@
       <c r="B62">
         <v>12</v>
       </c>
+      <c r="D62">
+        <v>13.05</v>
+      </c>
+      <c r="E62">
+        <v>12.2</v>
+      </c>
       <c r="G62">
         <v>12.2</v>
       </c>
@@ -1223,6 +1422,12 @@
       <c r="B63">
         <v>11.85</v>
       </c>
+      <c r="D63">
+        <v>11.6</v>
+      </c>
+      <c r="E63">
+        <v>12.1</v>
+      </c>
       <c r="G63">
         <v>11.867000000000001</v>
       </c>
@@ -1237,6 +1442,12 @@
       <c r="B64">
         <v>11.3</v>
       </c>
+      <c r="D64">
+        <v>11.35</v>
+      </c>
+      <c r="E64">
+        <v>12.1</v>
+      </c>
       <c r="G64">
         <v>11.867000000000001</v>
       </c>
@@ -1251,6 +1462,12 @@
       <c r="B65">
         <v>10.95</v>
       </c>
+      <c r="D65">
+        <v>11.05</v>
+      </c>
+      <c r="E65">
+        <v>11.3</v>
+      </c>
       <c r="G65">
         <v>11.6</v>
       </c>
@@ -1265,6 +1482,12 @@
       <c r="B66">
         <v>10.85</v>
       </c>
+      <c r="D66">
+        <v>11.05</v>
+      </c>
+      <c r="E66">
+        <v>11.25</v>
+      </c>
       <c r="G66">
         <v>10.967000000000001</v>
       </c>
@@ -1279,6 +1502,12 @@
       <c r="B67">
         <v>10.75</v>
       </c>
+      <c r="D67">
+        <v>10.6</v>
+      </c>
+      <c r="E67">
+        <v>10.3</v>
+      </c>
       <c r="G67">
         <v>10.9</v>
       </c>
@@ -1293,6 +1522,12 @@
       <c r="B68">
         <v>10</v>
       </c>
+      <c r="D68">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="E68">
+        <v>10.15</v>
+      </c>
       <c r="G68">
         <v>10.199999999999999</v>
       </c>
@@ -1307,19 +1542,23 @@
     </row>
     <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
+      <c r="D73" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="G73" s="6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -1329,6 +1568,12 @@
       <c r="B74">
         <v>11</v>
       </c>
+      <c r="D74">
+        <v>12</v>
+      </c>
+      <c r="E74">
+        <v>12.2</v>
+      </c>
       <c r="G74">
         <v>13.25</v>
       </c>
@@ -1343,6 +1588,12 @@
       <c r="B75">
         <v>11.45</v>
       </c>
+      <c r="D75">
+        <v>12.8</v>
+      </c>
+      <c r="E75">
+        <v>12.25</v>
+      </c>
       <c r="G75">
         <v>12.15</v>
       </c>
@@ -1357,6 +1608,12 @@
       <c r="B76">
         <v>11.2</v>
       </c>
+      <c r="D76">
+        <v>11.75</v>
+      </c>
+      <c r="E76">
+        <v>11.7</v>
+      </c>
       <c r="G76">
         <v>12.95</v>
       </c>
@@ -1371,6 +1628,12 @@
       <c r="B77">
         <v>11.35</v>
       </c>
+      <c r="D77">
+        <v>11.75</v>
+      </c>
+      <c r="E77">
+        <v>12.4</v>
+      </c>
       <c r="G77">
         <v>10.050000000000001</v>
       </c>
@@ -1385,6 +1648,12 @@
       <c r="B78">
         <v>11.55</v>
       </c>
+      <c r="D78">
+        <v>11.1</v>
+      </c>
+      <c r="E78">
+        <v>10.85</v>
+      </c>
       <c r="G78">
         <v>12.3</v>
       </c>
@@ -1399,6 +1668,12 @@
       <c r="B79">
         <v>11.25</v>
       </c>
+      <c r="D79">
+        <v>11.9</v>
+      </c>
+      <c r="E79">
+        <v>11.85</v>
+      </c>
       <c r="G79">
         <v>11.55</v>
       </c>
@@ -1413,6 +1688,12 @@
       <c r="B80">
         <v>9.1</v>
       </c>
+      <c r="D80">
+        <v>11.3</v>
+      </c>
+      <c r="E80">
+        <v>10</v>
+      </c>
       <c r="G80">
         <v>10.35</v>
       </c>
@@ -1427,6 +1708,12 @@
       <c r="B81">
         <v>11.1</v>
       </c>
+      <c r="D81">
+        <v>12.15</v>
+      </c>
+      <c r="E81">
+        <v>11.5</v>
+      </c>
       <c r="G81">
         <v>11.35</v>
       </c>
@@ -1441,6 +1728,12 @@
       <c r="B82">
         <v>11.7</v>
       </c>
+      <c r="D82">
+        <v>11</v>
+      </c>
+      <c r="E82">
+        <v>10.1</v>
+      </c>
       <c r="G82">
         <v>10.6</v>
       </c>
@@ -1455,6 +1748,12 @@
       <c r="B83">
         <v>11.75</v>
       </c>
+      <c r="D83">
+        <v>12.35</v>
+      </c>
+      <c r="E83">
+        <v>9.6</v>
+      </c>
       <c r="G83">
         <v>11.2</v>
       </c>
@@ -1469,6 +1768,12 @@
       <c r="B84">
         <v>10.050000000000001</v>
       </c>
+      <c r="D84">
+        <v>10.45</v>
+      </c>
+      <c r="E84">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="G84">
         <v>11.2</v>
       </c>
@@ -1483,6 +1788,12 @@
       <c r="B85">
         <v>9.75</v>
       </c>
+      <c r="D85">
+        <v>10</v>
+      </c>
+      <c r="E85">
+        <v>7.7</v>
+      </c>
       <c r="G85">
         <v>9.4</v>
       </c>
@@ -1497,6 +1808,12 @@
       <c r="B86">
         <v>10.35</v>
       </c>
+      <c r="D86">
+        <v>10.65</v>
+      </c>
+      <c r="E86">
+        <v>8.6999999999999993</v>
+      </c>
       <c r="G86">
         <v>11.05</v>
       </c>
@@ -1511,6 +1828,12 @@
       <c r="B87">
         <v>10.95</v>
       </c>
+      <c r="D87">
+        <v>11.35</v>
+      </c>
+      <c r="E87">
+        <v>12.4</v>
+      </c>
       <c r="G87">
         <v>9.65</v>
       </c>
@@ -1525,6 +1848,12 @@
       <c r="B88">
         <v>9.1</v>
       </c>
+      <c r="D88">
+        <v>10.5</v>
+      </c>
+      <c r="E88">
+        <v>9.85</v>
+      </c>
       <c r="G88">
         <v>11.2</v>
       </c>
@@ -1536,6 +1865,9 @@
       <c r="B89">
         <v>9.1999999999999993</v>
       </c>
+      <c r="D89">
+        <v>9.35</v>
+      </c>
       <c r="G89">
         <v>10.199999999999999</v>
       </c>
@@ -1547,6 +1879,9 @@
       <c r="B90">
         <v>10.25</v>
       </c>
+      <c r="D90">
+        <v>9.3000000000000007</v>
+      </c>
       <c r="G90">
         <v>10.4</v>
       </c>
@@ -1607,7 +1942,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B98" s="11"/>
       <c r="C98" s="11"/>
@@ -1619,19 +1954,23 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-      <c r="E99" s="6"/>
+      <c r="D99" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="G99" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H99" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -1641,6 +1980,12 @@
       <c r="B100">
         <v>47.1</v>
       </c>
+      <c r="D100">
+        <v>50.45</v>
+      </c>
+      <c r="E100">
+        <v>48.5</v>
+      </c>
       <c r="G100">
         <v>52.5</v>
       </c>
@@ -1655,6 +2000,12 @@
       <c r="B101">
         <v>46.484000000000002</v>
       </c>
+      <c r="D101">
+        <v>50.15</v>
+      </c>
+      <c r="E101">
+        <v>47.95</v>
+      </c>
       <c r="G101">
         <v>48.3</v>
       </c>
@@ -1669,6 +2020,12 @@
       <c r="B102">
         <v>45.466999999999999</v>
       </c>
+      <c r="D102">
+        <v>49.35</v>
+      </c>
+      <c r="E102">
+        <v>45.65</v>
+      </c>
       <c r="G102">
         <v>48.05</v>
       </c>
@@ -1683,6 +2040,12 @@
       <c r="B103">
         <v>45.267000000000003</v>
       </c>
+      <c r="D103">
+        <v>48.6</v>
+      </c>
+      <c r="E103">
+        <v>44.95</v>
+      </c>
       <c r="G103">
         <v>46.75</v>
       </c>
@@ -1697,6 +2060,12 @@
       <c r="B104">
         <v>44.933999999999997</v>
       </c>
+      <c r="D104">
+        <v>48.55</v>
+      </c>
+      <c r="E104">
+        <v>44.25</v>
+      </c>
       <c r="G104">
         <v>45.7</v>
       </c>
@@ -1711,6 +2080,12 @@
       <c r="B105">
         <v>44.917000000000002</v>
       </c>
+      <c r="D105">
+        <v>47.85</v>
+      </c>
+      <c r="E105">
+        <v>43.65</v>
+      </c>
       <c r="G105">
         <v>43.6</v>
       </c>
@@ -1725,6 +2100,12 @@
       <c r="B106">
         <v>43.366999999999997</v>
       </c>
+      <c r="D106">
+        <v>46.95</v>
+      </c>
+      <c r="E106">
+        <v>42.05</v>
+      </c>
       <c r="G106">
         <v>43.15</v>
       </c>
@@ -1739,6 +2120,12 @@
       <c r="B107">
         <v>43</v>
       </c>
+      <c r="D107">
+        <v>46.85</v>
+      </c>
+      <c r="E107">
+        <v>41.95</v>
+      </c>
       <c r="G107">
         <v>42.15</v>
       </c>
@@ -1753,6 +2140,12 @@
       <c r="B108">
         <v>42.634</v>
       </c>
+      <c r="D108">
+        <v>45.55</v>
+      </c>
+      <c r="E108">
+        <v>41</v>
+      </c>
       <c r="G108">
         <v>42.05</v>
       </c>
@@ -1767,6 +2160,12 @@
       <c r="B109">
         <v>42.616999999999997</v>
       </c>
+      <c r="D109">
+        <v>45.45</v>
+      </c>
+      <c r="E109">
+        <v>39.200000000000003</v>
+      </c>
       <c r="G109">
         <v>41.95</v>
       </c>
@@ -1781,6 +2180,12 @@
       <c r="B110">
         <v>42.2</v>
       </c>
+      <c r="D110">
+        <v>44.5</v>
+      </c>
+      <c r="E110">
+        <v>39.049999999999997</v>
+      </c>
       <c r="G110">
         <v>41.6</v>
       </c>
@@ -1795,6 +2200,12 @@
       <c r="B111">
         <v>41.85</v>
       </c>
+      <c r="D111">
+        <v>44.45</v>
+      </c>
+      <c r="E111">
+        <v>37.950000000000003</v>
+      </c>
       <c r="G111">
         <v>41.5</v>
       </c>
@@ -1806,6 +2217,12 @@
       <c r="B112">
         <v>40.35</v>
       </c>
+      <c r="D112">
+        <v>44.35</v>
+      </c>
+      <c r="E112">
+        <v>37.799999999999997</v>
+      </c>
       <c r="G112">
         <v>41.45</v>
       </c>
@@ -1817,6 +2234,9 @@
       <c r="B113">
         <v>37.799999999999997</v>
       </c>
+      <c r="D113">
+        <v>42.95</v>
+      </c>
       <c r="G113">
         <v>40.15</v>
       </c>
@@ -1827,6 +2247,9 @@
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>37.634</v>
+      </c>
+      <c r="D114">
+        <v>41.7</v>
       </c>
       <c r="G114">
         <v>35.15</v>
@@ -1905,12 +2328,16 @@
     </row>
     <row r="130" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B130" s="9"/>
       <c r="C130" s="8"/>
-      <c r="D130" s="8"/>
-      <c r="E130" s="8"/>
+      <c r="D130" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E130" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="F130" s="7"/>
       <c r="G130" s="7" t="s">
         <v>19</v>
@@ -1919,32 +2346,40 @@
         <v>20</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C131" s="7"/>
-      <c r="D131" s="7"/>
-      <c r="E131" s="7"/>
+      <c r="D131" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E131" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F131" s="7"/>
       <c r="G131" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="7">
         <v>13.625</v>
       </c>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
-      <c r="D132" s="7"/>
-      <c r="E132" s="7"/>
+      <c r="D132" s="13">
+        <v>12.85</v>
+      </c>
+      <c r="E132" s="13">
+        <v>12.45</v>
+      </c>
       <c r="F132" s="7"/>
       <c r="G132" s="7">
         <v>13.775</v>
@@ -1953,14 +2388,18 @@
         <v>12.574999999999999</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="7">
         <v>12.6</v>
       </c>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
-      <c r="D133" s="7"/>
-      <c r="E133" s="7"/>
+      <c r="D133" s="13">
+        <v>12.55</v>
+      </c>
+      <c r="E133" s="13">
+        <v>11.875</v>
+      </c>
       <c r="F133" s="7"/>
       <c r="G133" s="7">
         <v>13.574999999999999</v>
@@ -1969,14 +2408,18 @@
         <v>12.574999999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="7">
         <v>11.6</v>
       </c>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
-      <c r="D134" s="7"/>
-      <c r="E134" s="7"/>
+      <c r="D134" s="13">
+        <v>11.225</v>
+      </c>
+      <c r="E134" s="13">
+        <v>11.4</v>
+      </c>
       <c r="F134" s="7"/>
       <c r="G134" s="7">
         <v>13.4</v>
@@ -2056,24 +2499,36 @@
       <c r="H143" s="5"/>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G144" s="1"/>
+      <c r="A144" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D144" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G144" s="1">
+        <v>2022</v>
+      </c>
       <c r="H144" s="5"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C145" s="1"/>
-      <c r="D145" s="1"/>
-      <c r="E145" s="1"/>
+      <c r="D145" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="G145" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -2084,8 +2539,12 @@
         <v>6</v>
       </c>
       <c r="C146" s="1"/>
-      <c r="D146" s="1"/>
-      <c r="E146" s="1"/>
+      <c r="D146" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G146" s="1" t="s">
         <v>6</v>
       </c>
@@ -2100,6 +2559,12 @@
       <c r="B147">
         <v>12.65</v>
       </c>
+      <c r="D147">
+        <v>14.5</v>
+      </c>
+      <c r="E147">
+        <v>14.1</v>
+      </c>
       <c r="G147">
         <v>13.75</v>
       </c>
@@ -2114,6 +2579,12 @@
       <c r="B148">
         <v>12.75</v>
       </c>
+      <c r="D148">
+        <v>13.25</v>
+      </c>
+      <c r="E148">
+        <v>14.1</v>
+      </c>
       <c r="G148">
         <v>13.9</v>
       </c>
@@ -2128,6 +2599,12 @@
       <c r="B149">
         <v>13.7</v>
       </c>
+      <c r="D149">
+        <v>13.65</v>
+      </c>
+      <c r="E149">
+        <v>11.7</v>
+      </c>
       <c r="G149">
         <v>13.3</v>
       </c>
@@ -2142,6 +2619,12 @@
       <c r="B150">
         <v>11.1</v>
       </c>
+      <c r="D150">
+        <v>11.9</v>
+      </c>
+      <c r="E150">
+        <v>12.2</v>
+      </c>
       <c r="G150">
         <v>13.5</v>
       </c>
@@ -2153,6 +2636,12 @@
       <c r="A151">
         <v>13.25</v>
       </c>
+      <c r="D151">
+        <v>12.95</v>
+      </c>
+      <c r="E151">
+        <v>10.65</v>
+      </c>
       <c r="G151">
         <v>13.4</v>
       </c>
@@ -2161,6 +2650,12 @@
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D152">
+        <v>13.25</v>
+      </c>
+      <c r="E152">
+        <v>11.85</v>
+      </c>
       <c r="G152">
         <v>13.75</v>
       </c>
@@ -2192,7 +2687,6 @@
       <c r="G156">
         <v>13.95</v>
       </c>
-      <c r="H156" s="5"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G157" s="5">
@@ -2217,8 +2711,12 @@
         <v>20</v>
       </c>
       <c r="C162" s="1"/>
-      <c r="D162" s="1"/>
-      <c r="E162" s="1"/>
+      <c r="D162" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="G162" s="1" t="s">
         <v>19</v>
       </c>
@@ -2234,8 +2732,12 @@
         <v>21</v>
       </c>
       <c r="C163" s="1"/>
-      <c r="D163" s="1"/>
-      <c r="E163" s="1"/>
+      <c r="D163" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="G163" s="1" t="s">
         <v>21</v>
       </c>
@@ -2248,7 +2750,13 @@
         <v>14.5</v>
       </c>
       <c r="B164" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="D164">
+        <v>14.25</v>
+      </c>
+      <c r="E164">
+        <v>13.05</v>
       </c>
       <c r="G164">
         <v>13.45</v>
@@ -2262,7 +2770,13 @@
         <v>13.9</v>
       </c>
       <c r="B165" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="D165">
+        <v>13.35</v>
+      </c>
+      <c r="E165">
+        <v>13.05</v>
       </c>
       <c r="G165">
         <v>13.45</v>
@@ -2276,7 +2790,13 @@
         <v>12.7</v>
       </c>
       <c r="B166" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="D166">
+        <v>13.05</v>
+      </c>
+      <c r="E166">
+        <v>12.65</v>
       </c>
       <c r="G166">
         <v>11.4</v>
@@ -2290,7 +2810,13 @@
         <v>12.3</v>
       </c>
       <c r="B167" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="D167">
+        <v>8.75</v>
+      </c>
+      <c r="E167">
+        <v>11.45</v>
       </c>
       <c r="G167">
         <v>12.85</v>
@@ -2304,7 +2830,10 @@
         <v>11.5</v>
       </c>
       <c r="B168" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="E168">
+        <v>10.95</v>
       </c>
       <c r="G168">
         <v>12.25</v>
@@ -2318,7 +2847,10 @@
         <v>10.15</v>
       </c>
       <c r="B169" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="E169">
+        <v>10.7</v>
       </c>
       <c r="G169">
         <v>10.5</v>
@@ -2328,6 +2860,9 @@
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E170">
+        <v>8.8000000000000007</v>
+      </c>
       <c r="H170">
         <v>10.55</v>
       </c>
@@ -2339,19 +2874,23 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C173" s="1"/>
-      <c r="D173" s="1"/>
-      <c r="E173" s="1"/>
+      <c r="D173" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="G173" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H173" s="1" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
@@ -2361,6 +2900,12 @@
       <c r="B174">
         <v>13.5</v>
       </c>
+      <c r="D174">
+        <v>13.55</v>
+      </c>
+      <c r="E174">
+        <v>11.6</v>
+      </c>
       <c r="G174">
         <v>13.45</v>
       </c>
@@ -2375,6 +2920,12 @@
       <c r="B175">
         <v>12.4</v>
       </c>
+      <c r="D175">
+        <v>12.5</v>
+      </c>
+      <c r="E175">
+        <v>13.05</v>
+      </c>
       <c r="G175">
         <v>13.1</v>
       </c>
@@ -2389,6 +2940,12 @@
       <c r="B176">
         <v>12.7</v>
       </c>
+      <c r="D176">
+        <v>14.1</v>
+      </c>
+      <c r="E176">
+        <v>12.65</v>
+      </c>
       <c r="G176">
         <v>13.15</v>
       </c>
@@ -2403,6 +2960,12 @@
       <c r="B177">
         <v>8.5</v>
       </c>
+      <c r="D177">
+        <v>12.65</v>
+      </c>
+      <c r="E177">
+        <v>10.65</v>
+      </c>
       <c r="G177">
         <v>13.45</v>
       </c>
@@ -2414,6 +2977,12 @@
       <c r="A178">
         <v>13.4</v>
       </c>
+      <c r="D178">
+        <v>11.4</v>
+      </c>
+      <c r="E178">
+        <v>8.9</v>
+      </c>
       <c r="G178">
         <v>12.85</v>
       </c>
@@ -2422,6 +2991,9 @@
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D179">
+        <v>12.2</v>
+      </c>
       <c r="G179">
         <v>12.7</v>
       </c>
@@ -2544,12 +3116,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished FIG 2022 Score Comparison
</commit_message>
<xml_diff>
--- a/FIG-2022-Score-Comparison.xlsx
+++ b/FIG-2022-Score-Comparison.xlsx
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="56">
   <si>
     <t>WAG</t>
   </si>
   <si>
     <t>MAG</t>
-  </si>
-  <si>
-    <t>AA</t>
   </si>
   <si>
     <t>Floor</t>
@@ -149,9 +146,6 @@
     <t>MAG: Men's Artistic Gymnastics</t>
   </si>
   <si>
-    <t>AA: Overall</t>
-  </si>
-  <si>
     <t>1. Overall scores were included only if all 4 pieces of apparatus were competed on.</t>
   </si>
   <si>
@@ -170,9 +164,6 @@
     <t>Summary:</t>
   </si>
   <si>
-    <t xml:space="preserve">WAG Vault: </t>
-  </si>
-  <si>
     <t>Difference compared to year 2022. (Positive number means that year scored higher than 2022)</t>
   </si>
   <si>
@@ -183,6 +174,21 @@
   </si>
   <si>
     <t>Median</t>
+  </si>
+  <si>
+    <t>WAG Vault</t>
+  </si>
+  <si>
+    <t>WAG Beam</t>
+  </si>
+  <si>
+    <t>WAG Overall</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>MAG Floor</t>
   </si>
 </sst>
 </file>
@@ -323,7 +329,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -349,6 +355,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -638,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +672,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -676,7 +685,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>-0.5</v>
@@ -684,7 +693,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>-0.2</v>
@@ -692,7 +701,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>-0.4</v>
@@ -703,7 +712,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>-0.1</v>
@@ -713,24 +722,37 @@
       <c r="A7" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>48</v>
+      <c r="A9" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="15">
+      <c r="B11" s="17">
         <v>0.51012500000000216</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="C11" s="17">
+        <v>0.41862499999999869</v>
+      </c>
+      <c r="D11" s="17">
+        <v>2.4853750000000048</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0.19166666666666465</v>
+      </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -744,14 +766,20 @@
       <c r="R11" s="10"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="15">
+      <c r="B12" s="17">
         <v>0.51825000000000188</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="C12" s="17">
+        <v>0.43249999999999922</v>
+      </c>
+      <c r="D12" s="17">
+        <v>2.2675625000000039</v>
+      </c>
+      <c r="E12" s="17">
+        <v>3.3333333333333215E-2</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
@@ -765,14 +793,20 @@
       <c r="R12" s="10"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="15">
+      <c r="B13" s="17">
         <v>1.1372083333333336</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="C13" s="17">
+        <v>-0.13137500000000379</v>
+      </c>
+      <c r="D13" s="17">
+        <v>3.4539583333333468</v>
+      </c>
+      <c r="E13" s="17">
+        <v>-4.1071428571425983E-2</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -786,16 +820,18 @@
       <c r="R13" s="10"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="15">
+      <c r="B14" s="17">
         <v>-0.36612500000000026</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+      <c r="C14" s="17">
+        <v>0.65750000000000064</v>
+      </c>
+      <c r="D14" s="17">
+        <v>2.2590384615384664</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0.43783333333333552</v>
+      </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -807,14 +843,18 @@
       <c r="R14" s="10"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
+      <c r="B15" s="17">
         <v>0.26791666666666636</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="C15" s="17">
+        <v>0.44743589743589673</v>
+      </c>
+      <c r="D15" s="17">
+        <v>1.6203371481595781</v>
+      </c>
+      <c r="E15" s="17">
+        <v>1.0306666666666668</v>
+      </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -828,15 +868,18 @@
       <c r="R15" s="10"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
+      <c r="B16" s="17">
         <v>0.27200956937798892</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="C16" s="17">
+        <v>1.6142857142857139</v>
+      </c>
+      <c r="D16" s="17">
+        <v>1.0694291819291877</v>
+      </c>
+      <c r="E16" s="17">
+        <v>2.0209090909090932</v>
+      </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -849,14 +892,20 @@
       <c r="R16" s="10"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="4">
+      <c r="B17" s="17">
         <v>-0.33125000000000071</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="C17" s="17">
+        <v>0.29826086956521713</v>
+      </c>
+      <c r="D17" s="17">
+        <v>0.42651639344261838</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0.67738095238095042</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
@@ -870,121 +919,217 @@
       <c r="R17" s="10"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="4">
+      <c r="B18" s="17">
         <v>1.2772727272727273</v>
       </c>
+      <c r="C18" s="17">
+        <v>0.37297619047618902</v>
+      </c>
+      <c r="D18" s="17">
+        <v>1.4272435897435898</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0.62424242424242671</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="15">
+      <c r="B19" s="17">
         <v>0.71590109890109943</v>
       </c>
+      <c r="C19" s="17">
+        <v>0.1870843989769817</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17">
+        <v>0.27238095238095106</v>
+      </c>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="15">
+      <c r="B20" s="17">
         <v>0.19223529411764595</v>
       </c>
+      <c r="C20" s="17">
+        <v>0.60916666666666508</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17">
+        <v>6.2912912912912233E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="15">
+      <c r="B21" s="17">
         <v>0.58736263736264327</v>
       </c>
+      <c r="C21" s="17">
+        <v>0.65663594470045972</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17">
+        <v>-0.1914446002805068</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="15">
+      <c r="B22" s="17">
         <v>0.27461538461538559</v>
       </c>
+      <c r="C22" s="17">
+        <v>0.59178690344062623</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17">
+        <v>-0.27151486486486398</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="4">
+      <c r="B23" s="17">
         <v>0.39714861751152242</v>
       </c>
+      <c r="C23" s="17">
+        <v>0.33714285714285985</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17">
+        <v>0.50179211469534124</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="4">
+      <c r="B24" s="17">
         <v>0.42201257861635355</v>
       </c>
+      <c r="C24" s="17">
+        <v>0.69157681940700932</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
+      <c r="B25" s="17">
         <v>0.12383512544802855</v>
       </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
+      <c r="B26" s="17">
         <v>0.44721583064887582</v>
       </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27">
+      <c r="A27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="19">
         <f>AVERAGE(B11:B26)</f>
         <v>0.40285836649201712</v>
       </c>
+      <c r="C27" s="19">
+        <f>AVERAGE(C11:C26)</f>
+        <v>0.51311444729268663</v>
+      </c>
+      <c r="D27" s="19">
+        <f>AVERAGE(D11:D26)</f>
+        <v>1.8761825760183495</v>
+      </c>
+      <c r="E27" s="19">
+        <f>AVERAGE(E11:E26)</f>
+        <v>0.41146827336960601</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28">
+      <c r="A28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="19">
         <f>MEDIAN(B11:B26)</f>
         <v>0.40958059806393798</v>
       </c>
+      <c r="C28" s="19">
+        <f>MEDIAN(C11:C26)</f>
+        <v>0.43996794871794798</v>
+      </c>
+      <c r="D28" s="19">
+        <f>MEDIAN(D11:D26)</f>
+        <v>1.9396878048490223</v>
+      </c>
+      <c r="E28" s="19">
+        <f>MEDIAN(E11:E26)</f>
+        <v>0.27238095238095106</v>
+      </c>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="A34" s="5"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -994,43 +1139,43 @@
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K46" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="AE46" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AE48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K49" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AE49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.25">
@@ -1080,7 +1225,7 @@
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
@@ -1090,7 +1235,7 @@
       <c r="G52" s="12"/>
       <c r="H52" s="12"/>
       <c r="K52" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L52" s="12"/>
       <c r="M52" s="12"/>
@@ -1102,44 +1247,44 @@
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="K53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L53" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="M53" s="1"/>
       <c r="N53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O53" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="O53" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="P53" s="1"/>
       <c r="Q53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R53" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="R53" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.25">
@@ -1627,44 +1772,44 @@
     </row>
     <row r="77" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K77" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L77" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M77" s="6"/>
       <c r="N77" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O77" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P77" s="6"/>
       <c r="Q77" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R77" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
@@ -3377,7 +3522,7 @@
     <row r="168" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B170" s="12"/>
       <c r="C170" s="12"/>
@@ -3387,7 +3532,7 @@
       <c r="G170" s="12"/>
       <c r="H170" s="12"/>
       <c r="K170" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L170" s="12"/>
       <c r="M170" s="12"/>
@@ -3419,42 +3564,42 @@
     </row>
     <row r="172" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B172" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="B172" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="C172" s="6"/>
       <c r="D172" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G172" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H172" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H172" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="K172" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L172" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="L172" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="M172" s="6"/>
       <c r="N172" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O172" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q172" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="R172" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="R172" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.25">
@@ -3477,10 +3622,10 @@
         <v>12.567</v>
       </c>
       <c r="K173" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L173" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N173" s="10">
         <v>13.65</v>
@@ -3831,42 +3976,42 @@
     </row>
     <row r="192" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B192" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B192" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="C192" s="6"/>
       <c r="D192" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E192" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E192" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="G192" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H192" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H192" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="K192" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L192" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="L192" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="M192" s="6"/>
       <c r="N192" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O192" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O192" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="Q192" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R192" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="R192" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.25">
@@ -5695,7 +5840,7 @@
     </row>
     <row r="289" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A289" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B289" s="12"/>
       <c r="C289" s="12"/>
@@ -5705,7 +5850,7 @@
       <c r="G289" s="12"/>
       <c r="H289" s="12"/>
       <c r="K289" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L289" s="12"/>
       <c r="M289" s="12"/>
@@ -5741,42 +5886,42 @@
     </row>
     <row r="291" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A291" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B291" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="B291" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="C291" s="6"/>
       <c r="D291" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E291" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E291" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="G291" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H291" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H291" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="K291" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L291" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="L291" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="M291" s="6"/>
       <c r="N291" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O291" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O291" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="Q291" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R291" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="R291" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="292" spans="1:18" x14ac:dyDescent="0.25">
@@ -7477,86 +7622,86 @@
     </row>
     <row r="385" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A385" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B385" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="B385" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="C385" s="7"/>
       <c r="D385" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E385" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="E385" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="F385" s="7"/>
       <c r="G385" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H385" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H385" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="K385" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L385" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="L385" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="M385" s="7"/>
       <c r="N385" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O385" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="O385" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="P385" s="7"/>
       <c r="Q385" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="R385" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="R385" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="386" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A386" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B386" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C386" s="7"/>
       <c r="D386" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E386" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F386" s="7"/>
       <c r="G386" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H386" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K386" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L386" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M386" s="7"/>
       <c r="N386" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O386" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P386" s="7"/>
       <c r="Q386" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R386" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="387" spans="1:18" x14ac:dyDescent="0.25">
@@ -7564,7 +7709,7 @@
         <v>14.5</v>
       </c>
       <c r="B387" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D387">
         <v>14.25</v>
@@ -7579,10 +7724,10 @@
         <v>12.45</v>
       </c>
       <c r="K387" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L387" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N387" s="10">
         <v>14.333</v>
@@ -7602,7 +7747,7 @@
         <v>13.9</v>
       </c>
       <c r="B388" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D388">
         <v>13.35</v>
@@ -7634,7 +7779,7 @@
         <v>12.7</v>
       </c>
       <c r="B389" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D389">
         <v>13.05</v>
@@ -7666,7 +7811,7 @@
         <v>12.3</v>
       </c>
       <c r="B390" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D390">
         <v>8.75</v>
@@ -7698,7 +7843,7 @@
         <v>11.5</v>
       </c>
       <c r="B391" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E391">
         <v>10.95</v>
@@ -7727,7 +7872,7 @@
         <v>10.15</v>
       </c>
       <c r="B392" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E392">
         <v>10.7</v>
@@ -7894,86 +8039,86 @@
     </row>
     <row r="405" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A405" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B405" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="B405" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="C405" s="7"/>
       <c r="D405" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E405" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="E405" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="F405" s="7"/>
       <c r="G405" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H405" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H405" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="K405" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L405" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="L405" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="M405" s="7"/>
       <c r="N405" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O405" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="O405" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="P405" s="7"/>
       <c r="Q405" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="R405" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="R405" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="406" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A406" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B406" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C406" s="7"/>
       <c r="D406" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E406" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F406" s="7"/>
       <c r="G406" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H406" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K406" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L406" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M406" s="7"/>
       <c r="N406" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O406" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P406" s="7"/>
       <c r="Q406" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R406" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="407" spans="1:18" x14ac:dyDescent="0.25">
@@ -8791,12 +8936,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>